<commit_message>
mapa de procesos de 14
</commit_message>
<xml_diff>
--- a/01_Documentacion/1. Mapa de procesos/G2_MAPA_PROC_V2.xlsx
+++ b/01_Documentacion/1. Mapa de procesos/G2_MAPA_PROC_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14F5C319-2540-4291-A814-F0944EC15599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75FA9E65-F8D9-4888-AAEB-04A69117D64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4997B183-6BA5-427C-8615-A6F9FCD80629}"/>
   </bookViews>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">Integrantes </t>
   </si>
   <si>
+    <t>Jeimy Marley Morales Sosa</t>
+  </si>
+  <si>
     <t>Grupo:</t>
   </si>
   <si>
@@ -61,10 +64,19 @@
     <t>Ing. Jenny Ruiz</t>
   </si>
   <si>
+    <t>Steven Jefferson Pozo Analuisa</t>
+  </si>
+  <si>
+    <t>Erick Patricio Ramírez Ortíz</t>
+  </si>
+  <si>
     <t>NRC:</t>
   </si>
   <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sebastian Paúl Torres Tapia  </t>
   </si>
   <si>
     <t>Tema:</t>
@@ -147,18 +159,6 @@
   </si>
   <si>
     <t>NRC:              14569 / G·               estudiantes: Alexader Guacan, Milena Maldonado, Antoni Toapanta</t>
-  </si>
-  <si>
-    <t>Steven Jefferson Pozo Analuisa</t>
-  </si>
-  <si>
-    <t>Erick Patricio Ramírez Ortíz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sebastian Paúl Torres Tapia  </t>
-  </si>
-  <si>
-    <t>Jeimy Marley Morales Sosa</t>
   </si>
 </sst>
 </file>
@@ -306,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -326,17 +326,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -344,36 +367,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6709,7 +6705,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>482510</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>167697</xdr:rowOff>
+      <xdr:rowOff>167895</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
@@ -6734,8 +6730,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7835417" y="3600625"/>
-          <a:ext cx="9025" cy="726647"/>
+          <a:off x="7569110" y="3606420"/>
+          <a:ext cx="9025" cy="727628"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -10759,8 +10755,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3675512" y="5854890"/>
-          <a:ext cx="1145461" cy="497987"/>
+          <a:off x="3668477" y="5813618"/>
+          <a:ext cx="1142647" cy="495408"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15215,13 +15211,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>IEEE 29119</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-EC">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
+            <a:t>IEEE 829 </a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="es-EC" sz="1100">
               <a:solidFill>
@@ -15251,7 +15242,7 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>416586</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>160077</xdr:rowOff>
+      <xdr:rowOff>160275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
@@ -15276,8 +15267,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="11445947" y="3593005"/>
-          <a:ext cx="11344" cy="738077"/>
+          <a:off x="11046486" y="3598800"/>
+          <a:ext cx="11344" cy="739058"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -15456,13 +15447,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>IEEE 29119</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-EC">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
+            <a:t>IEEE 829 </a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="es-EC" sz="1100"/>
             <a:t>Especificación de Diseño de Pruebas</a:t>
@@ -15475,13 +15461,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>6866</xdr:colOff>
+      <xdr:colOff>17962</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>61096</xdr:rowOff>
+      <xdr:rowOff>60999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>18125</xdr:colOff>
+      <xdr:colOff>29221</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>161867</xdr:rowOff>
     </xdr:to>
@@ -15495,14 +15481,15 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="88" idx="2"/>
           <a:endCxn id="60" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20227361" y="3494024"/>
-          <a:ext cx="11259" cy="823492"/>
+          <a:off x="19506112" y="3499524"/>
+          <a:ext cx="11259" cy="824768"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -15681,13 +15668,11 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>IEEE 29119</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-EC">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
+            <a:t>IEEE 829</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
           <a:r>
             <a:rPr lang="es-EC" sz="1100"/>
             <a:t>Informe de Incidentes de Prueba</a:t>
@@ -15708,7 +15693,7 @@
       <xdr:col>44</xdr:col>
       <xdr:colOff>96420</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>4045</xdr:rowOff>
+      <xdr:rowOff>3751</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -15726,8 +15711,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="27055255" y="3552156"/>
-          <a:ext cx="1825" cy="788219"/>
+          <a:off x="26078795" y="3557753"/>
+          <a:ext cx="1825" cy="789398"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -15922,14 +15907,27 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>IEEE 29119</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-EC" sz="1000">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+            <a:t>IEEE 829</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="es-US" sz="1000">
               <a:solidFill>
@@ -15950,14 +15948,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>610181</xdr:colOff>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>8534</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>90947</xdr:rowOff>
+      <xdr:rowOff>90869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>47</xdr:col>
-      <xdr:colOff>15708</xdr:colOff>
+      <xdr:colOff>26805</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>9837</xdr:rowOff>
     </xdr:to>
@@ -15971,14 +15969,15 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="117" idx="2"/>
           <a:endCxn id="63" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28796325" y="3523875"/>
-          <a:ext cx="18270" cy="822292"/>
+          <a:off x="27764384" y="3529394"/>
+          <a:ext cx="18271" cy="823843"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -24922,10 +24921,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -25270,10 +25265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8B49B5-0ECE-4555-B935-30B61D398401}">
-  <dimension ref="C1:AF103"/>
+  <dimension ref="C2:AF103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA125" sqref="AA125"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="97" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AX18" sqref="AX18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25281,171 +25276,170 @@
     <col min="14" max="15" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="16:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="16:32" x14ac:dyDescent="0.3">
-      <c r="P2" s="9"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="11" t="s">
+      <c r="P2" s="10"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="12"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="21"/>
     </row>
     <row r="3" spans="16:32" x14ac:dyDescent="0.3">
-      <c r="P3" s="13"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="16"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="17"/>
     </row>
     <row r="4" spans="16:32" x14ac:dyDescent="0.3">
-      <c r="P4" s="13"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="15" t="s">
+      <c r="P4" s="12"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15" t="s">
+      <c r="S4" s="16"/>
+      <c r="T4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB4" s="15" t="s">
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="AC4" s="15" t="s">
+      <c r="AB4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AD4" s="15" t="s">
+      <c r="AC4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AE4" s="15"/>
-      <c r="AF4" s="16"/>
+      <c r="AD4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="17"/>
     </row>
     <row r="5" spans="16:32" x14ac:dyDescent="0.3">
-      <c r="P5" s="13"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15" t="s">
-        <v>35</v>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16" t="s">
+        <v>7</v>
       </c>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="17"/>
     </row>
     <row r="6" spans="16:32" x14ac:dyDescent="0.3">
-      <c r="P6" s="13"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15" t="s">
-        <v>36</v>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16" t="s">
+        <v>8</v>
       </c>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15" t="s">
-        <v>6</v>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16" t="s">
+        <v>9</v>
       </c>
-      <c r="AB6" s="15">
+      <c r="AB6" s="16">
         <v>2567</v>
       </c>
-      <c r="AC6" s="15" t="s">
-        <v>7</v>
+      <c r="AC6" s="16" t="s">
+        <v>10</v>
       </c>
-      <c r="AD6" s="17">
+      <c r="AD6" s="18">
         <v>45614</v>
       </c>
-      <c r="AE6" s="17"/>
-      <c r="AF6" s="18"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="16:32" x14ac:dyDescent="0.3">
-      <c r="P7" s="13"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15" t="s">
-        <v>37</v>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16" t="s">
+        <v>11</v>
       </c>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15"/>
-      <c r="AA7" s="15"/>
-      <c r="AB7" s="15"/>
-      <c r="AC7" s="15"/>
-      <c r="AD7" s="17"/>
-      <c r="AE7" s="17"/>
-      <c r="AF7" s="18"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
+      <c r="AF7" s="19"/>
     </row>
-    <row r="8" spans="16:32" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="P8" s="19"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20" t="s">
-        <v>8</v>
+    <row r="8" spans="16:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P8" s="14"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15" t="s">
+        <v>12</v>
       </c>
-      <c r="S8" s="20"/>
-      <c r="T8" s="21" t="s">
-        <v>9</v>
+      <c r="S8" s="15"/>
+      <c r="T8" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="24"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="9"/>
     </row>
     <row r="17" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="18" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -25525,25 +25519,25 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AC4:AC5"/>
     <mergeCell ref="AD4:AF5"/>
     <mergeCell ref="AB6:AB7"/>
     <mergeCell ref="AC6:AC7"/>
     <mergeCell ref="AD6:AF7"/>
+    <mergeCell ref="P2:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="AA4:AA5"/>
+    <mergeCell ref="AA6:AA7"/>
+    <mergeCell ref="AB4:AB5"/>
     <mergeCell ref="R2:AF3"/>
     <mergeCell ref="R4:S7"/>
     <mergeCell ref="T4:Z4"/>
     <mergeCell ref="T5:Z5"/>
     <mergeCell ref="T6:Z6"/>
     <mergeCell ref="T7:Z7"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="AA4:AA5"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="AB4:AB5"/>
-    <mergeCell ref="AC4:AC5"/>
-    <mergeCell ref="P2:Q8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="26" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="26" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="51" max="116" man="1"/>
   </colBreaks>
@@ -25576,37 +25570,37 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:50" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
-        <v>10</v>
+      <c r="B2" s="22" t="s">
+        <v>14</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
       <c r="AE2" s="5"/>
       <c r="AF2" s="5"/>
       <c r="AG2" s="5"/>
@@ -25630,67 +25624,67 @@
     </row>
     <row r="3" spans="1:50" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
     </row>
     <row r="4" spans="1:50" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
     </row>
     <row r="5" spans="1:50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -25757,7 +25751,7 @@
     <row r="10" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -25767,7 +25761,7 @@
     <row r="11" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -25790,17 +25784,17 @@
     <row r="14" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>14</v>
+      <c r="A15" s="16" t="s">
+        <v>18</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
@@ -25818,13 +25812,13 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="L17" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="AF17" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -25856,13 +25850,13 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="AO21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -25870,21 +25864,21 @@
       <c r="AC22" s="3"/>
     </row>
     <row r="23" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>18</v>
+      <c r="A23" s="16" t="s">
+        <v>22</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="O23" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="Y23" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="AI23" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -25910,7 +25904,7 @@
     <row r="27" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -25919,7 +25913,7 @@
     <row r="28" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -25935,18 +25929,18 @@
     <row r="30" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>23</v>
+      <c r="A31" s="16" t="s">
+        <v>27</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
@@ -25960,7 +25954,7 @@
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -25969,7 +25963,7 @@
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -25985,18 +25979,18 @@
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
-        <v>27</v>
+      <c r="A37" s="16" t="s">
+        <v>31</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
@@ -26010,7 +26004,7 @@
     <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -26019,7 +26013,7 @@
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -26035,7 +26029,7 @@
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -26044,7 +26038,7 @@
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -26079,13 +26073,13 @@
     <row r="51" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -26095,99 +26089,99 @@
     <row r="57" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B60" s="8" t="s">
-        <v>34</v>
+      <c r="B60" s="22" t="s">
+        <v>38</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
-      <c r="L60" s="8"/>
-      <c r="M60" s="8"/>
-      <c r="N60" s="8"/>
-      <c r="O60" s="8"/>
-      <c r="P60" s="8"/>
-      <c r="Q60" s="8"/>
-      <c r="R60" s="8"/>
-      <c r="S60" s="8"/>
-      <c r="T60" s="8"/>
-      <c r="U60" s="8"/>
-      <c r="V60" s="8"/>
-      <c r="W60" s="8"/>
-      <c r="X60" s="8"/>
-      <c r="Y60" s="8"/>
-      <c r="Z60" s="8"/>
-      <c r="AA60" s="8"/>
-      <c r="AB60" s="8"/>
-      <c r="AC60" s="8"/>
-      <c r="AD60" s="8"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="22"/>
+      <c r="L60" s="22"/>
+      <c r="M60" s="22"/>
+      <c r="N60" s="22"/>
+      <c r="O60" s="22"/>
+      <c r="P60" s="22"/>
+      <c r="Q60" s="22"/>
+      <c r="R60" s="22"/>
+      <c r="S60" s="22"/>
+      <c r="T60" s="22"/>
+      <c r="U60" s="22"/>
+      <c r="V60" s="22"/>
+      <c r="W60" s="22"/>
+      <c r="X60" s="22"/>
+      <c r="Y60" s="22"/>
+      <c r="Z60" s="22"/>
+      <c r="AA60" s="22"/>
+      <c r="AB60" s="22"/>
+      <c r="AC60" s="22"/>
+      <c r="AD60" s="22"/>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
-      <c r="L61" s="8"/>
-      <c r="M61" s="8"/>
-      <c r="N61" s="8"/>
-      <c r="O61" s="8"/>
-      <c r="P61" s="8"/>
-      <c r="Q61" s="8"/>
-      <c r="R61" s="8"/>
-      <c r="S61" s="8"/>
-      <c r="T61" s="8"/>
-      <c r="U61" s="8"/>
-      <c r="V61" s="8"/>
-      <c r="W61" s="8"/>
-      <c r="X61" s="8"/>
-      <c r="Y61" s="8"/>
-      <c r="Z61" s="8"/>
-      <c r="AA61" s="8"/>
-      <c r="AB61" s="8"/>
-      <c r="AC61" s="8"/>
-      <c r="AD61" s="8"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="22"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="22"/>
+      <c r="K61" s="22"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="22"/>
+      <c r="N61" s="22"/>
+      <c r="O61" s="22"/>
+      <c r="P61" s="22"/>
+      <c r="Q61" s="22"/>
+      <c r="R61" s="22"/>
+      <c r="S61" s="22"/>
+      <c r="T61" s="22"/>
+      <c r="U61" s="22"/>
+      <c r="V61" s="22"/>
+      <c r="W61" s="22"/>
+      <c r="X61" s="22"/>
+      <c r="Y61" s="22"/>
+      <c r="Z61" s="22"/>
+      <c r="AA61" s="22"/>
+      <c r="AB61" s="22"/>
+      <c r="AC61" s="22"/>
+      <c r="AD61" s="22"/>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="8"/>
-      <c r="M62" s="8"/>
-      <c r="N62" s="8"/>
-      <c r="O62" s="8"/>
-      <c r="P62" s="8"/>
-      <c r="Q62" s="8"/>
-      <c r="R62" s="8"/>
-      <c r="S62" s="8"/>
-      <c r="T62" s="8"/>
-      <c r="U62" s="8"/>
-      <c r="V62" s="8"/>
-      <c r="W62" s="8"/>
-      <c r="X62" s="8"/>
-      <c r="Y62" s="8"/>
-      <c r="Z62" s="8"/>
-      <c r="AA62" s="8"/>
-      <c r="AB62" s="8"/>
-      <c r="AC62" s="8"/>
-      <c r="AD62" s="8"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="22"/>
+      <c r="I62" s="22"/>
+      <c r="J62" s="22"/>
+      <c r="K62" s="22"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="22"/>
+      <c r="N62" s="22"/>
+      <c r="O62" s="22"/>
+      <c r="P62" s="22"/>
+      <c r="Q62" s="22"/>
+      <c r="R62" s="22"/>
+      <c r="S62" s="22"/>
+      <c r="T62" s="22"/>
+      <c r="U62" s="22"/>
+      <c r="V62" s="22"/>
+      <c r="W62" s="22"/>
+      <c r="X62" s="22"/>
+      <c r="Y62" s="22"/>
+      <c r="Z62" s="22"/>
+      <c r="AA62" s="22"/>
+      <c r="AB62" s="22"/>
+      <c r="AC62" s="22"/>
+      <c r="AD62" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -26205,23 +26199,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6130c624-bec2-48a0-a4e0-dd56eb2f89c2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004E0ED12E3C12264BAAEFDDE265025732" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2d362b695837bcdd23b5ff1cf77f037c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6130c624-bec2-48a0-a4e0-dd56eb2f89c2" xmlns:ns4="42803d71-5b3b-4609-9095-d55998e15ed0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4b59103f32c4b737153175474b0bd2f" ns3:_="" ns4:_="">
     <xsd:import namespace="6130c624-bec2-48a0-a4e0-dd56eb2f89c2"/>
@@ -26416,32 +26393,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B1EF6FC-E1A3-4516-8546-CCE0DBDE9A84}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="42803d71-5b3b-4609-9095-d55998e15ed0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6130c624-bec2-48a0-a4e0-dd56eb2f89c2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DF3A800-A648-4ED0-9604-A7A2B88DC5AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6130c624-bec2-48a0-a4e0-dd56eb2f89c2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA509352-82F5-4E08-96D0-34C8F7BC5A84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26458,4 +26427,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DF3A800-A648-4ED0-9604-A7A2B88DC5AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B1EF6FC-E1A3-4516-8546-CCE0DBDE9A84}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="6130c624-bec2-48a0-a4e0-dd56eb2f89c2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="42803d71-5b3b-4609-9095-d55998e15ed0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>